<commit_message>
LMS-2340 Finished implementing changes to templates and handlers.
SVN: 21890
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Proteomics-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/Proteomics-Example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>One of CE, ES, ME, CY, or NC</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -145,6 +145,10 @@
   </si>
   <si>
     <t>TIME::VALUE_TYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/TEST/TEST/TEST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -567,7 +571,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -592,7 +596,9 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -664,9 +670,9 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="3" max="1048575" man="1"/>
   </colBreaks>
@@ -753,6 +759,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
CCS-7, SP-30 Updated proteomics handlers to expect format template from Rolf
SVN: 25373
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Proteomics-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/Proteomics-Example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21105"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22221"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3260" yWindow="220" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
@@ -86,32 +86,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>One of mM, uM, Percent, RatioT1, RatioCs, or AU, Dimensionless</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>uM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GeneLocus</t>
   </si>
   <si>
     <t>HumanReadable</t>
   </si>
   <si>
-    <t>0::Mean</t>
-  </si>
-  <si>
-    <t>0::Std</t>
-  </si>
-  <si>
-    <t>+2100::Mean</t>
-  </si>
-  <si>
-    <t>+2100::Std</t>
-  </si>
-  <si>
     <t>BSU18500</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -149,6 +129,24 @@
   </si>
   <si>
     <t>JJS-MGP90</t>
+  </si>
+  <si>
+    <t>One of mM, uM, Percent, RatioT1, RatioCs, or AU, Dimensionless, fmol/ug protein digest</t>
+  </si>
+  <si>
+    <t>fmol/ug protein digest</t>
+  </si>
+  <si>
+    <t>0::Mean::B1_B2::T1_T2</t>
+  </si>
+  <si>
+    <t>0::Std::B1_B2::T1_T2</t>
+  </si>
+  <si>
+    <t>+2100::Mean::B1_B2::T1_T2</t>
+  </si>
+  <si>
+    <t>+2100::Std::B1_B2::T1_T2</t>
   </si>
 </sst>
 </file>
@@ -228,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -238,6 +236,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,14 +569,14 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="90" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20">
@@ -596,7 +595,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -607,7 +606,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
@@ -640,10 +639,10 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -651,7 +650,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
@@ -659,13 +658,13 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -687,41 +686,45 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>8.5510613820000003</v>
@@ -738,10 +741,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>11.461723579999999</v>

</xml_diff>

<commit_message>
CCS-7, SP-30 Finalized proteomics format
SVN: 25376
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Proteomics-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/Proteomics-Example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>One of CE, ES, ME, CY, or NC</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,10 +82,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>One of Lin, Log2, Log10, or Ln</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GeneLocus</t>
   </si>
   <si>
@@ -131,12 +127,6 @@
     <t>JJS-MGP90</t>
   </si>
   <si>
-    <t>One of mM, uM, Percent, RatioT1, RatioCs, or AU, Dimensionless, fmol/ug protein digest</t>
-  </si>
-  <si>
-    <t>fmol/ug protein digest</t>
-  </si>
-  <si>
     <t>0::Mean::B1_B2::T1_T2</t>
   </si>
   <si>
@@ -147,6 +137,18 @@
   </si>
   <si>
     <t>+2100::Std::B1_B2::T1_T2</t>
+  </si>
+  <si>
+    <t>Reference Strain</t>
+  </si>
+  <si>
+    <t>The Reference Strain (for relative quantification data sets, leave empty for absolute)</t>
+  </si>
+  <si>
+    <t>fmol/ug</t>
+  </si>
+  <si>
+    <t>One of mM, uM, Percent, RatioT1, RatioCs, AU, Dimensionless, fmol/ug</t>
   </si>
 </sst>
 </file>
@@ -566,15 +568,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="90" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -595,7 +597,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -606,7 +608,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
@@ -614,57 +616,64 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B4" s="5"/>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -701,30 +710,30 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>8.5510613820000003</v>
@@ -741,10 +750,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>11.461723579999999</v>

</xml_diff>